<commit_message>
final version project proposal
</commit_message>
<xml_diff>
--- a/COMP2501_Project/COMP2501_project_idea.xlsx
+++ b/COMP2501_Project/COMP2501_project_idea.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17320" windowHeight="16940"/>
+    <workbookView windowWidth="24980" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1012,15 +1012,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1494,13 +1497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1512,19 +1515,19 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:16">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1532,930 +1535,925 @@
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" hidden="1" customHeight="1" spans="1:16">
-      <c r="A3" s="4" t="s">
+    <row r="3" customHeight="1" spans="1:16">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="5"/>
       <c r="P3"/>
     </row>
-    <row r="4" hidden="1" customHeight="1" spans="1:16">
-      <c r="A4" s="4" t="s">
+    <row r="4" customHeight="1" spans="1:16">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="5"/>
       <c r="P4"/>
     </row>
-    <row r="5" hidden="1" customHeight="1" spans="1:4">
-      <c r="A5" s="4" t="s">
+    <row r="5" customHeight="1" spans="1:4">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" hidden="1" customHeight="1" spans="1:5">
-      <c r="A6" s="4" t="s">
+    <row r="6" customHeight="1" spans="1:5">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" hidden="1" customHeight="1" spans="1:5">
-      <c r="A7" s="4" t="s">
+    <row r="7" customHeight="1" spans="1:5">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" hidden="1" customHeight="1" spans="1:5">
-      <c r="A8" s="4" t="s">
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:16">
-      <c r="A11" s="5" t="s">
+    <row r="11" s="2" customFormat="1" customHeight="1" spans="1:16">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" hidden="1" customHeight="1" spans="1:5">
-      <c r="A12" s="5" t="s">
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" hidden="1" customHeight="1" spans="1:5">
-      <c r="A13" s="4" t="s">
+    <row r="13" customHeight="1" spans="1:5">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" hidden="1" customHeight="1" spans="1:5">
-      <c r="A14" s="4" t="s">
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" hidden="1" customHeight="1" spans="1:5">
-      <c r="A15" s="4" t="s">
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" hidden="1" customHeight="1" spans="1:5">
-      <c r="A16" s="4" t="s">
+    <row r="16" customHeight="1" spans="1:5">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" hidden="1" customHeight="1" spans="1:5">
-      <c r="A17" s="4" t="s">
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" hidden="1" customHeight="1" spans="1:5">
-      <c r="A18" s="4" t="s">
+    <row r="18" customHeight="1" spans="1:5">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" hidden="1" customHeight="1" spans="1:5">
-      <c r="A19" s="4" t="s">
+    <row r="19" customHeight="1" spans="1:5">
+      <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" hidden="1" customHeight="1" spans="1:16">
-      <c r="A20" s="5" t="s">
+    <row r="20" s="2" customFormat="1" customHeight="1" spans="1:16">
+      <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A21" s="5" t="s">
+    <row r="21" s="2" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:5">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" hidden="1" customHeight="1" spans="1:16">
-      <c r="A24" s="4" t="s">
+    <row r="24" customHeight="1" spans="1:16">
+      <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="5"/>
       <c r="P24"/>
     </row>
-    <row r="25" hidden="1" customHeight="1" spans="1:4">
-      <c r="A25" s="4" t="s">
+    <row r="25" customHeight="1" spans="1:4">
+      <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" hidden="1" customHeight="1" spans="1:4">
-      <c r="A26" s="4" t="s">
+    <row r="26" customHeight="1" spans="1:4">
+      <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" hidden="1" customHeight="1" spans="1:5">
-      <c r="A27" s="4" t="s">
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" customHeight="1" spans="1:16">
-      <c r="A28" s="6" t="s">
+    <row r="28" s="3" customFormat="1" customHeight="1" spans="1:16">
+      <c r="A28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="P28" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" hidden="1" customHeight="1" spans="1:16">
-      <c r="A29" s="4" t="s">
+    <row r="29" customHeight="1" spans="1:16">
+      <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="5"/>
       <c r="P29"/>
     </row>
-    <row r="30" hidden="1" customHeight="1" spans="1:16">
-      <c r="A30" s="4" t="s">
+    <row r="30" customHeight="1" spans="1:16">
+      <c r="A30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="5"/>
       <c r="P30"/>
     </row>
-    <row r="31" hidden="1" customHeight="1" spans="1:16">
-      <c r="A31" s="4" t="s">
+    <row r="31" customHeight="1" spans="1:16">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="5"/>
       <c r="P31"/>
     </row>
-    <row r="32" hidden="1" customHeight="1" spans="1:16">
-      <c r="A32" s="4" t="s">
+    <row r="32" customHeight="1" spans="1:16">
+      <c r="A32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="5"/>
       <c r="P32"/>
     </row>
-    <row r="33" hidden="1" customHeight="1" spans="1:16">
-      <c r="A33" s="4" t="s">
+    <row r="33" customHeight="1" spans="1:16">
+      <c r="A33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="5"/>
       <c r="P33"/>
     </row>
-    <row r="34" s="2" customFormat="1" customHeight="1" spans="1:16">
-      <c r="A34" s="6" t="s">
+    <row r="34" s="3" customFormat="1" customHeight="1" spans="1:16">
+      <c r="A34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="P34" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:5">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" hidden="1" customHeight="1" spans="1:16">
-      <c r="A37" s="4" t="s">
+    <row r="37" customHeight="1" spans="1:16">
+      <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="5"/>
       <c r="P37"/>
     </row>
-    <row r="38" hidden="1" customHeight="1" spans="1:16">
-      <c r="A38" s="4" t="s">
+    <row r="38" customHeight="1" spans="1:16">
+      <c r="A38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="5"/>
       <c r="P38"/>
     </row>
-    <row r="39" hidden="1" customHeight="1" spans="1:4">
-      <c r="A39" s="4" t="s">
+    <row r="39" customHeight="1" spans="1:4">
+      <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" hidden="1" customHeight="1" spans="1:16">
-      <c r="A40" s="4" t="s">
+    <row r="40" customHeight="1" spans="1:16">
+      <c r="A40" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="5"/>
       <c r="P40"/>
     </row>
     <row r="41" customHeight="1" spans="1:5">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="1:5">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" hidden="1" customHeight="1" spans="1:16">
-      <c r="A43" s="4" t="s">
+    <row r="43" customHeight="1" spans="1:16">
+      <c r="A43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="5"/>
       <c r="P43"/>
     </row>
-    <row r="44" hidden="1" customHeight="1" spans="1:16">
-      <c r="A44" s="4" t="s">
+    <row r="44" customHeight="1" spans="1:16">
+      <c r="A44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="5"/>
       <c r="P44"/>
     </row>
-    <row r="45" hidden="1" customHeight="1" spans="1:16">
-      <c r="A45" s="4" t="s">
+    <row r="45" customHeight="1" spans="1:16">
+      <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="5"/>
       <c r="P45"/>
     </row>
-    <row r="46" hidden="1" customHeight="1" spans="1:16">
-      <c r="A46" s="4" t="s">
+    <row r="46" customHeight="1" spans="1:16">
+      <c r="A46" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="5"/>
       <c r="P46"/>
     </row>
-    <row r="47" hidden="1" customHeight="1" spans="1:5">
-      <c r="A47" s="4" t="s">
+    <row r="47" customHeight="1" spans="1:5">
+      <c r="A47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" hidden="1" customHeight="1" spans="1:5">
-      <c r="A48" s="4" t="s">
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" hidden="1" customHeight="1" spans="1:5">
-      <c r="A49" s="4" t="s">
+    <row r="49" customHeight="1" spans="1:5">
+      <c r="A49" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="50" customHeight="1" spans="1:5">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:5">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" hidden="1" customHeight="1" spans="1:16">
-      <c r="A52" s="4" t="s">
+    <row r="52" customHeight="1" spans="1:16">
+      <c r="A52" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="5"/>
       <c r="P52"/>
     </row>
-    <row r="53" hidden="1" customHeight="1" spans="1:16">
-      <c r="A53" s="4" t="s">
+    <row r="53" customHeight="1" spans="1:16">
+      <c r="A53" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="5"/>
       <c r="P53"/>
     </row>
-    <row r="54" hidden="1" customHeight="1" spans="1:5">
-      <c r="A54" s="4" t="s">
+    <row r="54" customHeight="1" spans="1:5">
+      <c r="A54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" hidden="1" customHeight="1" spans="1:5">
-      <c r="A55" s="4" t="s">
+    <row r="55" customHeight="1" spans="1:5">
+      <c r="A55" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" hidden="1" customHeight="1" spans="1:5">
-      <c r="A56" s="4" t="s">
+    <row r="56" customHeight="1" spans="1:5">
+      <c r="A56" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="9" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B1:B56" etc:filterBottomFollowUsedRange="0">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="equal" val="Aosaf"/>
-      </customFilters>
-    </filterColumn>
     <extLst/>
   </autoFilter>
   <mergeCells count="4">
@@ -2471,7 +2469,7 @@
     <hyperlink ref="E11" r:id="rId4" display="https://www.kaggle.com/datasets/datasnaek/mbti-type"/>
     <hyperlink ref="E12" r:id="rId5" display="https://www.kaggle.com/datasets/sidraaazam/graduate-employability-dataset"/>
     <hyperlink ref="E13" r:id="rId6" display="https://archive.ics.uci.edu/dataset/544/estimation+of+obesity+levels+based+on+eating+habits+and+physical+condition"/>
-    <hyperlink ref="E14" r:id="rId7" display="https://www.kaggle.com/datasets/afnansaifafnan/study-habits-and-activities-of-students"/>
+    <hyperlink ref="E14" r:id="rId7" display="https://www.kaggle.com/datasets/afnansaifafnan/study-habits-and-activities-of-students" tooltip="https://www.kaggle.com/datasets/afnansaifafnan/study-habits-and-activities-of-students"/>
     <hyperlink ref="E15" r:id="rId8" display="https://www.kaggle.com/datasets/prince7489/mental-health-and-social-media-balance-dataset"/>
     <hyperlink ref="E16" r:id="rId9" display="https://www.kaggle.com/datasets/miadul/lifestyle-and-health-risk-prediction"/>
     <hyperlink ref="E17" r:id="rId10" display="https://www.kaggle.com/datasets/nalisha/student-exam-scores-analysis-ipyn"/>

</xml_diff>